<commit_message>
Boogie: Added a new code snippet for IEnumerable out parameters
</commit_message>
<xml_diff>
--- a/Util/Code Snippets/Code snippet documentation.xlsx
+++ b/Util/Code Snippets/Code snippet documentation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
   <si>
     <t>Title</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Out value that must not be null</t>
+  </si>
+  <si>
+    <t>Contract.Ensures(cce.NonNullElements(Contract.ValueAtReturn(...)))</t>
+  </si>
+  <si>
+    <t>cernn</t>
   </si>
 </sst>
 </file>
@@ -618,7 +624,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -963,6 +969,35 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1010,7 +1045,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1024,31 +1059,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1391,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,24 +1456,24 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
@@ -1449,12 +1483,12 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1464,12 +1498,12 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -1479,12 +1513,12 @@
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1494,12 +1528,12 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1509,12 +1543,12 @@
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
@@ -1524,12 +1558,12 @@
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1539,12 +1573,12 @@
       <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1554,12 +1588,12 @@
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1569,12 +1603,12 @@
       <c r="D11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -1584,12 +1618,12 @@
       <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="6" t="s">
         <v>43</v>
       </c>
@@ -1599,12 +1633,12 @@
       <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="6" t="s">
         <v>47</v>
       </c>
@@ -1614,12 +1648,12 @@
       <c r="D14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="6" t="s">
         <v>50</v>
       </c>
@@ -1629,12 +1663,12 @@
       <c r="D15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="6" t="s">
         <v>54</v>
       </c>
@@ -1644,12 +1678,12 @@
       <c r="D16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="6" t="s">
         <v>58</v>
       </c>
@@ -1659,12 +1693,12 @@
       <c r="D17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="6" t="s">
         <v>61</v>
       </c>
@@ -1674,44 +1708,44 @@
       <c r="D18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="6" t="s">
         <v>74</v>
       </c>
@@ -1721,12 +1755,12 @@
       <c r="D21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="6" t="s">
         <v>78</v>
       </c>
@@ -1736,12 +1770,12 @@
       <c r="D22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="6" t="s">
         <v>82</v>
       </c>
@@ -1751,12 +1785,12 @@
       <c r="D23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="6" t="s">
         <v>85</v>
       </c>
@@ -1766,29 +1800,38 @@
       <c r="D24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="13" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A19"/>
-    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A20:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>